<commit_message>
Added price/volatility jump to DGP + noise + README
</commit_message>
<xml_diff>
--- a/result_testing/tests.xlsx
+++ b/result_testing/tests.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\totna\Dokumentumok\Jupyter\Jump_Code\result_testing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B8EFEE4-8488-4386-9E28-E3F88DC94AB6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33528844-9E78-4314-9E4F-41A51F89FAFD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="21820" windowHeight="14020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="10800" windowHeight="13800" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -177,7 +177,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="23">
+  <borders count="19">
     <border>
       <left/>
       <right/>
@@ -333,56 +333,6 @@
         <color auto="1"/>
       </top>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="dashed">
-        <color auto="1"/>
-      </right>
-      <top/>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="dashed">
-        <color indexed="64"/>
-      </left>
-      <right style="dashed">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="dashed">
-        <color auto="1"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="dashed">
-        <color auto="1"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -501,41 +451,41 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -908,7 +858,7 @@
   <dimension ref="B1:H14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F27" sqref="F27"/>
+      <selection activeCell="H14" sqref="B14:H14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -926,24 +876,24 @@
   <sheetData>
     <row r="1" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="2" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B2" s="23" t="s">
+      <c r="B2" s="18" t="s">
         <v>24</v>
       </c>
-      <c r="C2" s="24"/>
-      <c r="D2" s="24"/>
-      <c r="E2" s="24"/>
-      <c r="F2" s="24"/>
-      <c r="G2" s="24"/>
-      <c r="H2" s="25"/>
+      <c r="C2" s="19"/>
+      <c r="D2" s="19"/>
+      <c r="E2" s="19"/>
+      <c r="F2" s="19"/>
+      <c r="G2" s="19"/>
+      <c r="H2" s="20"/>
     </row>
     <row r="3" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B3" s="26"/>
-      <c r="C3" s="27"/>
-      <c r="D3" s="27"/>
-      <c r="E3" s="27"/>
-      <c r="F3" s="27"/>
-      <c r="G3" s="27"/>
-      <c r="H3" s="28"/>
+      <c r="B3" s="21"/>
+      <c r="C3" s="22"/>
+      <c r="D3" s="22"/>
+      <c r="E3" s="22"/>
+      <c r="F3" s="22"/>
+      <c r="G3" s="22"/>
+      <c r="H3" s="23"/>
     </row>
     <row r="4" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B4" s="7" t="s">
@@ -1143,7 +1093,7 @@
       <c r="C12" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="D12" s="22" t="s">
+      <c r="D12" s="17" t="s">
         <v>22</v>
       </c>
       <c r="E12" s="4">
@@ -1160,7 +1110,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="13" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="13" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B13" s="13" t="s">
         <v>15</v>
       </c>
@@ -1185,26 +1135,26 @@
       </c>
     </row>
     <row r="14" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B14" s="17" t="s">
+      <c r="B14" s="24" t="s">
         <v>18</v>
       </c>
-      <c r="C14" s="18" t="s">
+      <c r="C14" s="25" t="s">
         <v>19</v>
       </c>
-      <c r="D14" s="19" t="s">
-        <v>3</v>
-      </c>
-      <c r="E14" s="18">
+      <c r="D14" s="26" t="s">
+        <v>3</v>
+      </c>
+      <c r="E14" s="25">
         <v>93</v>
       </c>
-      <c r="F14" s="20">
+      <c r="F14" s="27">
         <v>79</v>
       </c>
-      <c r="G14" s="20">
+      <c r="G14" s="27">
         <f t="shared" si="0"/>
         <v>14</v>
       </c>
-      <c r="H14" s="21" t="s">
+      <c r="H14" s="28" t="s">
         <v>3</v>
       </c>
     </row>

</xml_diff>